<commit_message>
debugging; next step is to debug lure on special branch.
</commit_message>
<xml_diff>
--- a/config/xlsx/fish_pond.xlsx
+++ b/config/xlsx/fish_pond.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="29868" windowHeight="13500" firstSheet="1" activeTab="1"/>
+    <workbookView windowHeight="18240" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="HookConst" sheetId="9" state="hidden" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="59">
   <si>
     <t>INT64</t>
   </si>
@@ -125,43 +125,40 @@
     <t>[OpenSpot]#5</t>
   </si>
   <si>
-    <t>RO_Lake</t>
+    <t>Noob_Lake</t>
+  </si>
+  <si>
+    <t>ro01_area_2D</t>
+  </si>
+  <si>
+    <t>item_currency_coins</t>
+  </si>
+  <si>
+    <t>NULL</t>
+  </si>
+  <si>
+    <t>金币</t>
+  </si>
+  <si>
+    <t>Ogle_Lake</t>
+  </si>
+  <si>
+    <t>ogle01_area_2D</t>
+  </si>
+  <si>
+    <t>raven_lake</t>
+  </si>
+  <si>
+    <t>raven01_2D</t>
+  </si>
+  <si>
+    <t>raven01_area_2D</t>
+  </si>
+  <si>
+    <t>Roe_River</t>
   </si>
   <si>
     <t>ro01_2D</t>
-  </si>
-  <si>
-    <t>ro01_area_2D</t>
-  </si>
-  <si>
-    <t>item_currency_coins</t>
-  </si>
-  <si>
-    <t>NULL</t>
-  </si>
-  <si>
-    <t>金币</t>
-  </si>
-  <si>
-    <t>ogle_lake</t>
-  </si>
-  <si>
-    <t>ogle01_2D</t>
-  </si>
-  <si>
-    <t>ogle01_area_2D</t>
-  </si>
-  <si>
-    <t>raven_lake</t>
-  </si>
-  <si>
-    <t>raven01_2D</t>
-  </si>
-  <si>
-    <t>raven01_area_2D</t>
-  </si>
-  <si>
-    <t>Roe_River</t>
   </si>
   <si>
     <t>DOUBLE</t>
@@ -915,9 +912,6 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -926,6 +920,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -1275,12 +1272,12 @@
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.87962962962963" defaultRowHeight="13.8" outlineLevelRow="2" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="8.88333333333333" defaultRowHeight="14.25" outlineLevelRow="2" outlineLevelCol="4"/>
   <cols>
     <col min="2" max="2" width="28" customWidth="1"/>
-    <col min="3" max="3" width="39.3796296296296" customWidth="1"/>
+    <col min="3" max="3" width="39.3833333333333" customWidth="1"/>
     <col min="4" max="4" width="23" customWidth="1"/>
-    <col min="5" max="5" width="23.1296296296296" customWidth="1"/>
+    <col min="5" max="5" width="23.1333333333333" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -1358,18 +1355,18 @@
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="H22" sqref="H22"/>
+      <selection pane="bottomRight" activeCell="A5" sqref="A5:C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" outlineLevelRow="7"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="7"/>
   <cols>
-    <col min="1" max="2" width="12.1296296296296" customWidth="1"/>
-    <col min="3" max="4" width="22.1296296296296" customWidth="1"/>
-    <col min="5" max="5" width="26.8796296296296" customWidth="1"/>
-    <col min="6" max="6" width="18.6296296296296" customWidth="1"/>
-    <col min="7" max="9" width="19.8796296296296" customWidth="1"/>
+    <col min="1" max="2" width="12.1333333333333" customWidth="1"/>
+    <col min="3" max="4" width="22.1333333333333" customWidth="1"/>
+    <col min="5" max="5" width="26.8833333333333" customWidth="1"/>
+    <col min="6" max="6" width="18.6333333333333" customWidth="1"/>
+    <col min="7" max="9" width="19.8833333333333" customWidth="1"/>
     <col min="10" max="12" width="32" style="12" customWidth="1"/>
-    <col min="13" max="13" width="18.6296296296296" customWidth="1"/>
+    <col min="13" max="13" width="18.6333333333333" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
@@ -1460,7 +1457,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" ht="27.6" spans="1:14">
+    <row r="3" ht="28.5" spans="1:14">
       <c r="A3" s="5" t="s">
         <v>2</v>
       </c>
@@ -1536,41 +1533,41 @@
       <c r="B5" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="C5" s="17" t="s">
+      <c r="C5" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" s="17" t="s">
         <v>32</v>
-      </c>
-      <c r="D5" s="18" t="s">
-        <v>33</v>
       </c>
       <c r="E5" s="5">
         <v>1</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G5" s="8">
         <v>0</v>
       </c>
-      <c r="H5" s="19">
+      <c r="H5" s="18">
         <v>1</v>
       </c>
       <c r="I5" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J5" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K5" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L5" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M5" s="5">
         <v>190</v>
       </c>
       <c r="N5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:14">
@@ -1578,24 +1575,24 @@
         <v>301020001</v>
       </c>
       <c r="B6" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6" s="17" t="s">
         <v>37</v>
-      </c>
-      <c r="C6" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="D6" s="18" t="s">
-        <v>39</v>
       </c>
       <c r="E6" s="5">
         <v>1</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G6" s="8">
         <v>0</v>
       </c>
-      <c r="H6" s="19">
+      <c r="H6" s="18">
         <v>1</v>
       </c>
       <c r="I6" s="8">
@@ -1608,13 +1605,13 @@
         <v>4</v>
       </c>
       <c r="L6" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M6" s="5">
         <v>140</v>
       </c>
       <c r="N6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:14">
@@ -1622,27 +1619,27 @@
         <v>301020002</v>
       </c>
       <c r="B7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7" t="s">
         <v>40</v>
-      </c>
-      <c r="C7" t="s">
-        <v>41</v>
-      </c>
-      <c r="D7" t="s">
-        <v>42</v>
       </c>
       <c r="E7">
         <v>21</v>
       </c>
       <c r="F7" t="s">
-        <v>34</v>
-      </c>
-      <c r="G7" s="20">
+        <v>33</v>
+      </c>
+      <c r="G7" s="19">
         <v>1200</v>
       </c>
-      <c r="H7" s="20">
+      <c r="H7" s="19">
         <v>1</v>
       </c>
-      <c r="I7" s="20">
+      <c r="I7" s="19">
         <v>2</v>
       </c>
       <c r="J7" s="8">
@@ -1658,7 +1655,7 @@
         <v>120</v>
       </c>
       <c r="N7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:14">
@@ -1666,27 +1663,27 @@
         <v>301020003</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="C8" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="D8" s="17" t="s">
         <v>32</v>
-      </c>
-      <c r="D8" s="18" t="s">
-        <v>33</v>
       </c>
       <c r="E8">
         <v>22</v>
       </c>
       <c r="F8" t="s">
-        <v>34</v>
-      </c>
-      <c r="G8" s="20">
+        <v>33</v>
+      </c>
+      <c r="G8" s="19">
         <v>3000</v>
       </c>
-      <c r="H8" s="20">
+      <c r="H8" s="19">
         <v>1</v>
       </c>
-      <c r="I8" s="20">
+      <c r="I8" s="19">
         <v>2</v>
       </c>
       <c r="J8" s="8">
@@ -1702,7 +1699,7 @@
         <v>120</v>
       </c>
       <c r="N8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -1754,7 +1751,7 @@
     <dataValidation type="custom" allowBlank="1" showErrorMessage="1" errorTitle="拒绝重复输入" error="当前输入的内容，与本区域的其他单元格内容重复。" sqref="C4:D4 C7:D7 C9:D1048576" errorStyle="warning">
       <formula1>COUNTIF(#REF!,C4)&lt;2</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showErrorMessage="1" errorTitle="拒绝重复输入" error="当前输入的内容，与本区域的其他单元格内容重复。" sqref="A9:B1048576 A1:B4 A5:B8" errorStyle="warning">
+    <dataValidation type="custom" allowBlank="1" showErrorMessage="1" errorTitle="拒绝重复输入" error="当前输入的内容，与本区域的其他单元格内容重复。" sqref="A$1:B$1048576" errorStyle="warning">
       <formula1>COUNTIF($A:$A,A1)&lt;2</formula1>
     </dataValidation>
   </dataValidations>
@@ -1773,14 +1770,14 @@
       <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.87962962962963" defaultRowHeight="13.8" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="8.88333333333333" defaultRowHeight="14.25" outlineLevelCol="5"/>
   <cols>
-    <col min="1" max="1" width="24.8796296296296" customWidth="1"/>
-    <col min="2" max="2" width="43.1296296296296" customWidth="1"/>
+    <col min="1" max="1" width="24.8833333333333" customWidth="1"/>
+    <col min="2" max="2" width="43.1333333333333" customWidth="1"/>
     <col min="3" max="3" width="23" customWidth="1"/>
-    <col min="4" max="4" width="20.1296296296296" customWidth="1"/>
+    <col min="4" max="4" width="20.1333333333333" customWidth="1"/>
     <col min="5" max="5" width="30.25" customWidth="1"/>
-    <col min="6" max="6" width="24.3796296296296" customWidth="1"/>
+    <col min="6" max="6" width="24.3833333333333" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -1797,10 +1794,10 @@
         <v>8</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -1811,16 +1808,16 @@
         <v>9</v>
       </c>
       <c r="C2" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="E2" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="F2" s="4" t="s">
         <v>47</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -1828,19 +1825,19 @@
         <v>2</v>
       </c>
       <c r="B3" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="D3" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="E3" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="F3" s="4" t="s">
         <v>52</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -1856,7 +1853,7 @@
         <v>301030000</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C5" s="9">
         <v>0.208333333333333</v>
@@ -1876,7 +1873,7 @@
         <v>301030001</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C6" s="9">
         <v>0.208333333333333</v>
@@ -1896,7 +1893,7 @@
         <v>301030002</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C7" s="9">
         <v>0.208333333333333</v>
@@ -1916,7 +1913,7 @@
         <v>900000000</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C8" s="9">
         <v>0.208333333333333</v>
@@ -1936,7 +1933,7 @@
         <v>301030100</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C9" s="9">
         <v>0.208333333333333</v>
@@ -1956,7 +1953,7 @@
         <v>301030101</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C10" s="9">
         <v>0.208333333333333</v>

</xml_diff>